<commit_message>
nascosto l'URL delle credenziali del database in settings.py e configurata la variabile ambientale di accordo con quella salvata su heroku
</commit_message>
<xml_diff>
--- a/uploaded_files/uploaded_glossaries/dati_da_app_glossario_gestisco.xlsx
+++ b/uploaded_files/uploaded_glossaries/dati_da_app_glossario_gestisco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommaso\Django rest framework\Udemy Django\Metaglossario_Gestisco\uploaded_files\uploaded_glossaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D7F8B5-A523-4CB1-BCC6-1B0E96F7E20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A6C26F-B75D-463F-A446-72221EF46201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="1930" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="434">
   <si>
     <t>Lemma</t>
   </si>
@@ -626,9 +626,6 @@
   </si>
   <si>
     <t>Vigili del fuoco</t>
-  </si>
-  <si>
-    <t>VVFF</t>
   </si>
   <si>
     <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
@@ -2227,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA0F904-3C69-4BAA-B8F3-98A1762B4AA2}">
   <dimension ref="A1:XFD77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="N76" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2248,7 +2245,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2275,16 +2272,16 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -18684,13 +18681,13 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
+        <v>317</v>
+      </c>
+      <c r="N2" t="s">
         <v>318</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>319</v>
-      </c>
-      <c r="O2" t="s">
-        <v>320</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -18725,13 +18722,13 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -18766,13 +18763,13 @@
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P4">
         <v>3</v>
@@ -18807,13 +18804,13 @@
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P5">
         <v>4</v>
@@ -18842,13 +18839,13 @@
         <v>36</v>
       </c>
       <c r="M6" t="s">
+        <v>323</v>
+      </c>
+      <c r="N6" t="s">
         <v>324</v>
       </c>
-      <c r="N6" t="s">
-        <v>325</v>
-      </c>
       <c r="O6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P6">
         <v>5</v>
@@ -18877,13 +18874,13 @@
         <v>43</v>
       </c>
       <c r="M7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -18909,13 +18906,13 @@
         <v>49</v>
       </c>
       <c r="M8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P8">
         <v>7</v>
@@ -18941,13 +18938,13 @@
         <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P9">
         <v>8</v>
@@ -18982,13 +18979,13 @@
         <v>49</v>
       </c>
       <c r="M10" t="s">
+        <v>328</v>
+      </c>
+      <c r="N10" t="s">
         <v>329</v>
       </c>
-      <c r="N10" t="s">
-        <v>330</v>
-      </c>
       <c r="O10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P10">
         <v>9</v>
@@ -19014,13 +19011,13 @@
         <v>49</v>
       </c>
       <c r="M11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P11">
         <v>10</v>
@@ -19046,13 +19043,13 @@
         <v>49</v>
       </c>
       <c r="M12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P12">
         <v>11</v>
@@ -19081,13 +19078,13 @@
         <v>71</v>
       </c>
       <c r="M13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P13">
         <v>12</v>
@@ -19116,13 +19113,13 @@
         <v>78</v>
       </c>
       <c r="M14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P14">
         <v>13</v>
@@ -19148,13 +19145,13 @@
         <v>49</v>
       </c>
       <c r="M15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P15">
         <v>14</v>
@@ -19180,13 +19177,13 @@
         <v>86</v>
       </c>
       <c r="M16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P16">
         <v>15</v>
@@ -19215,13 +19212,13 @@
         <v>36</v>
       </c>
       <c r="M17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P17">
         <v>16</v>
@@ -19250,13 +19247,13 @@
         <v>97</v>
       </c>
       <c r="M18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P18">
         <v>17</v>
@@ -19282,13 +19279,13 @@
         <v>86</v>
       </c>
       <c r="M19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P19">
         <v>18</v>
@@ -19314,13 +19311,13 @@
         <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P20">
         <v>19</v>
@@ -19349,13 +19346,13 @@
         <v>71</v>
       </c>
       <c r="M21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P21">
         <v>20</v>
@@ -19381,13 +19378,13 @@
         <v>43</v>
       </c>
       <c r="M22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P22">
         <v>21</v>
@@ -19422,13 +19419,13 @@
         <v>19</v>
       </c>
       <c r="M23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P23">
         <v>22</v>
@@ -19451,13 +19448,13 @@
         <v>116</v>
       </c>
       <c r="M24" t="s">
+        <v>343</v>
+      </c>
+      <c r="N24" t="s">
         <v>344</v>
       </c>
-      <c r="N24" t="s">
-        <v>345</v>
-      </c>
       <c r="O24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P24">
         <v>23</v>
@@ -19492,13 +19489,13 @@
         <v>19</v>
       </c>
       <c r="M25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P25">
         <v>24</v>
@@ -19509,7 +19506,7 @@
         <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C26" t="s">
         <v>122</v>
@@ -19536,13 +19533,13 @@
         <v>19</v>
       </c>
       <c r="M26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P26">
         <v>25</v>
@@ -19553,7 +19550,7 @@
         <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C27" t="s">
         <v>126</v>
@@ -19577,13 +19574,13 @@
         <v>19</v>
       </c>
       <c r="M27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P27">
         <v>26</v>
@@ -19594,7 +19591,7 @@
         <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C28" t="s">
         <v>129</v>
@@ -19621,13 +19618,13 @@
         <v>19</v>
       </c>
       <c r="M28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P28">
         <v>27</v>
@@ -19668,13 +19665,13 @@
         <v>135</v>
       </c>
       <c r="M29" t="s">
+        <v>349</v>
+      </c>
+      <c r="N29" t="s">
         <v>350</v>
       </c>
-      <c r="N29" t="s">
-        <v>351</v>
-      </c>
       <c r="O29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P29">
         <v>28</v>
@@ -19691,13 +19688,13 @@
         <v>133</v>
       </c>
       <c r="M30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P30">
         <v>29</v>
@@ -19714,13 +19711,13 @@
         <v>140</v>
       </c>
       <c r="M31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P31">
         <v>30</v>
@@ -19746,13 +19743,13 @@
         <v>145</v>
       </c>
       <c r="M32" t="s">
+        <v>353</v>
+      </c>
+      <c r="N32" t="s">
         <v>354</v>
       </c>
-      <c r="N32" t="s">
-        <v>355</v>
-      </c>
       <c r="O32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P32">
         <v>31</v>
@@ -19784,13 +19781,13 @@
         <v>19</v>
       </c>
       <c r="M33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P33">
         <v>32</v>
@@ -19825,13 +19822,13 @@
         <v>19</v>
       </c>
       <c r="M34" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P34">
         <v>33</v>
@@ -19866,13 +19863,13 @@
         <v>19</v>
       </c>
       <c r="M35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="O35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P35">
         <v>34</v>
@@ -19913,13 +19910,13 @@
         <v>161</v>
       </c>
       <c r="M36" t="s">
+        <v>358</v>
+      </c>
+      <c r="N36" t="s">
         <v>359</v>
       </c>
-      <c r="N36" t="s">
-        <v>360</v>
-      </c>
       <c r="O36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P36">
         <v>35</v>
@@ -19960,13 +19957,13 @@
         <v>162</v>
       </c>
       <c r="M37" t="s">
+        <v>360</v>
+      </c>
+      <c r="N37" t="s">
         <v>361</v>
       </c>
-      <c r="N37" t="s">
-        <v>362</v>
-      </c>
       <c r="O37" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P37">
         <v>36</v>
@@ -19995,13 +19992,13 @@
         <v>168</v>
       </c>
       <c r="M38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P38">
         <v>37</v>
@@ -20027,13 +20024,13 @@
         <v>174</v>
       </c>
       <c r="M39" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P39">
         <v>38</v>
@@ -20056,13 +20053,13 @@
         <v>178</v>
       </c>
       <c r="M40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="O40" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P40">
         <v>39</v>
@@ -20100,13 +20097,13 @@
         <v>184</v>
       </c>
       <c r="M41" t="s">
+        <v>364</v>
+      </c>
+      <c r="N41" t="s">
         <v>365</v>
       </c>
-      <c r="N41" t="s">
-        <v>366</v>
-      </c>
       <c r="O41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P41">
         <v>40</v>
@@ -20138,13 +20135,13 @@
         <v>192</v>
       </c>
       <c r="M42" t="s">
+        <v>366</v>
+      </c>
+      <c r="N42" t="s">
         <v>367</v>
       </c>
-      <c r="N42" t="s">
-        <v>368</v>
-      </c>
       <c r="O42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P42">
         <v>41</v>
@@ -20170,13 +20167,13 @@
         <v>197</v>
       </c>
       <c r="M43" t="s">
+        <v>368</v>
+      </c>
+      <c r="N43" t="s">
         <v>369</v>
       </c>
-      <c r="N43" t="s">
-        <v>370</v>
-      </c>
       <c r="O43" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P43">
         <v>42</v>
@@ -20187,19 +20184,19 @@
         <v>198</v>
       </c>
       <c r="B44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" t="s">
         <v>199</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>200</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F44" t="s">
         <v>201</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>202</v>
-      </c>
-      <c r="G44" t="s">
-        <v>203</v>
       </c>
       <c r="H44" t="s">
         <v>16</v>
@@ -20214,16 +20211,16 @@
         <v>183</v>
       </c>
       <c r="L44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P44">
         <v>43</v>
@@ -20234,22 +20231,22 @@
         <v>198</v>
       </c>
       <c r="B45" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" t="s">
         <v>205</v>
       </c>
-      <c r="C45" t="s">
+      <c r="I45" t="s">
         <v>206</v>
       </c>
-      <c r="I45" t="s">
-        <v>207</v>
-      </c>
       <c r="M45" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O45" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P45">
         <v>44</v>
@@ -20257,31 +20254,31 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" t="s">
         <v>208</v>
-      </c>
-      <c r="C46" t="s">
-        <v>209</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>
       </c>
       <c r="F46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J46" t="s">
         <v>48</v>
       </c>
       <c r="K46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M46" t="s">
+        <v>372</v>
+      </c>
+      <c r="N46" t="s">
         <v>373</v>
       </c>
-      <c r="N46" t="s">
-        <v>374</v>
-      </c>
       <c r="O46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P46">
         <v>45</v>
@@ -20289,37 +20286,37 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" t="s">
         <v>212</v>
-      </c>
-      <c r="D47" t="s">
-        <v>213</v>
       </c>
       <c r="E47" t="s">
         <v>133</v>
       </c>
       <c r="F47" t="s">
+        <v>213</v>
+      </c>
+      <c r="H47" t="s">
         <v>214</v>
-      </c>
-      <c r="H47" t="s">
-        <v>215</v>
       </c>
       <c r="I47" t="s">
         <v>133</v>
       </c>
       <c r="L47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M47" t="s">
+        <v>374</v>
+      </c>
+      <c r="N47" t="s">
         <v>375</v>
       </c>
-      <c r="N47" t="s">
-        <v>376</v>
-      </c>
       <c r="O47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P47">
         <v>46</v>
@@ -20330,31 +20327,31 @@
         <v>125</v>
       </c>
       <c r="B48" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>218</v>
       </c>
-      <c r="D48" t="s">
+      <c r="H48" t="s">
         <v>219</v>
       </c>
-      <c r="H48" t="s">
+      <c r="J48" t="s">
         <v>220</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>221</v>
       </c>
-      <c r="K48" t="s">
-        <v>222</v>
-      </c>
       <c r="M48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P48">
         <v>47</v>
@@ -20362,34 +20359,34 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C49" t="s">
+        <v>222</v>
+      </c>
+      <c r="F49" t="s">
         <v>223</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>224</v>
       </c>
-      <c r="H49" t="s">
+      <c r="J49" t="s">
         <v>225</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>226</v>
-      </c>
-      <c r="K49" t="s">
-        <v>227</v>
       </c>
       <c r="L49" t="s">
         <v>135</v>
       </c>
       <c r="M49" t="s">
+        <v>349</v>
+      </c>
+      <c r="N49" t="s">
         <v>350</v>
       </c>
-      <c r="N49" t="s">
-        <v>351</v>
-      </c>
       <c r="O49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P49">
         <v>48</v>
@@ -20400,34 +20397,34 @@
         <v>156</v>
       </c>
       <c r="C50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
       </c>
       <c r="F50" t="s">
+        <v>228</v>
+      </c>
+      <c r="H50" t="s">
         <v>229</v>
       </c>
-      <c r="H50" t="s">
+      <c r="J50" t="s">
+        <v>225</v>
+      </c>
+      <c r="K50" t="s">
         <v>230</v>
-      </c>
-      <c r="J50" t="s">
-        <v>226</v>
-      </c>
-      <c r="K50" t="s">
-        <v>231</v>
       </c>
       <c r="L50" t="s">
         <v>161</v>
       </c>
       <c r="M50" t="s">
+        <v>358</v>
+      </c>
+      <c r="N50" t="s">
         <v>359</v>
       </c>
-      <c r="N50" t="s">
-        <v>360</v>
-      </c>
       <c r="O50" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P50">
         <v>49</v>
@@ -20435,40 +20432,40 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D51" t="s">
         <v>56</v>
       </c>
       <c r="F51" t="s">
+        <v>232</v>
+      </c>
+      <c r="H51" t="s">
         <v>233</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
+        <v>225</v>
+      </c>
+      <c r="J51" t="s">
+        <v>225</v>
+      </c>
+      <c r="K51" t="s">
         <v>234</v>
-      </c>
-      <c r="I51" t="s">
-        <v>226</v>
-      </c>
-      <c r="J51" t="s">
-        <v>226</v>
-      </c>
-      <c r="K51" t="s">
-        <v>235</v>
       </c>
       <c r="L51" t="s">
         <v>162</v>
       </c>
       <c r="M51" t="s">
+        <v>360</v>
+      </c>
+      <c r="N51" t="s">
         <v>361</v>
       </c>
-      <c r="N51" t="s">
-        <v>362</v>
-      </c>
       <c r="O51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P51">
         <v>50</v>
@@ -20476,40 +20473,40 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C52" t="s">
+        <v>235</v>
+      </c>
+      <c r="E52" t="s">
         <v>236</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>237</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>238</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>239</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>240</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>241</v>
-      </c>
-      <c r="K52" t="s">
-        <v>242</v>
       </c>
       <c r="L52" t="s">
         <v>184</v>
       </c>
       <c r="M52" t="s">
+        <v>364</v>
+      </c>
+      <c r="N52" t="s">
         <v>365</v>
       </c>
-      <c r="N52" t="s">
-        <v>366</v>
-      </c>
       <c r="O52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P52">
         <v>51</v>
@@ -20517,37 +20514,37 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F53" t="s">
+        <v>237</v>
+      </c>
+      <c r="H53" t="s">
         <v>238</v>
       </c>
-      <c r="H53" t="s">
-        <v>239</v>
-      </c>
       <c r="J53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N53" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O53" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P53">
         <v>52</v>
@@ -20555,37 +20552,37 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
       </c>
       <c r="E54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F54" t="s">
+        <v>213</v>
+      </c>
+      <c r="H54" t="s">
         <v>214</v>
       </c>
-      <c r="H54" t="s">
-        <v>215</v>
-      </c>
       <c r="I54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M54" t="s">
+        <v>372</v>
+      </c>
+      <c r="N54" t="s">
         <v>373</v>
       </c>
-      <c r="N54" t="s">
-        <v>374</v>
-      </c>
       <c r="O54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P54">
         <v>54</v>
@@ -20593,34 +20590,34 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C55" t="s">
+        <v>245</v>
+      </c>
+      <c r="F55" t="s">
         <v>246</v>
       </c>
-      <c r="F55" t="s">
+      <c r="H55" t="s">
         <v>247</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>248</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
+        <v>220</v>
+      </c>
+      <c r="K55" t="s">
         <v>249</v>
       </c>
-      <c r="J55" t="s">
-        <v>221</v>
-      </c>
-      <c r="K55" t="s">
-        <v>250</v>
-      </c>
       <c r="M55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P55">
         <v>55</v>
@@ -20628,28 +20625,28 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C56" t="s">
+        <v>250</v>
+      </c>
+      <c r="H56" t="s">
         <v>251</v>
       </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
+        <v>220</v>
+      </c>
+      <c r="K56" t="s">
         <v>252</v>
       </c>
-      <c r="J56" t="s">
-        <v>221</v>
-      </c>
-      <c r="K56" t="s">
-        <v>253</v>
-      </c>
       <c r="M56" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N56" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P56">
         <v>56</v>
@@ -20657,34 +20654,34 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C57" t="s">
+        <v>253</v>
+      </c>
+      <c r="F57" t="s">
         <v>254</v>
       </c>
-      <c r="F57" t="s">
-        <v>255</v>
-      </c>
       <c r="H57" t="s">
+        <v>247</v>
+      </c>
+      <c r="I57" t="s">
         <v>248</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
+        <v>220</v>
+      </c>
+      <c r="K57" t="s">
         <v>249</v>
       </c>
-      <c r="J57" t="s">
-        <v>221</v>
-      </c>
-      <c r="K57" t="s">
-        <v>250</v>
-      </c>
       <c r="M57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N57" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P57">
         <v>57</v>
@@ -20692,34 +20689,34 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B58" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" t="s">
         <v>256</v>
-      </c>
-      <c r="C58" t="s">
-        <v>257</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
       </c>
       <c r="H58" t="s">
+        <v>257</v>
+      </c>
+      <c r="J58" t="s">
+        <v>220</v>
+      </c>
+      <c r="K58" t="s">
         <v>258</v>
       </c>
-      <c r="J58" t="s">
-        <v>221</v>
-      </c>
-      <c r="K58" t="s">
-        <v>259</v>
-      </c>
       <c r="M58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N58" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O58" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P58">
         <v>58</v>
@@ -20727,31 +20724,31 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
       </c>
       <c r="H59" t="s">
+        <v>260</v>
+      </c>
+      <c r="J59" t="s">
+        <v>220</v>
+      </c>
+      <c r="K59" t="s">
         <v>261</v>
       </c>
-      <c r="J59" t="s">
-        <v>221</v>
-      </c>
-      <c r="K59" t="s">
-        <v>262</v>
-      </c>
       <c r="M59" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N59" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O59" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P59">
         <v>59</v>
@@ -20759,34 +20756,34 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C60" t="s">
+        <v>262</v>
+      </c>
+      <c r="F60" t="s">
         <v>263</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
+        <v>224</v>
+      </c>
+      <c r="I60" t="s">
+        <v>248</v>
+      </c>
+      <c r="J60" t="s">
+        <v>225</v>
+      </c>
+      <c r="K60" t="s">
         <v>264</v>
       </c>
-      <c r="H60" t="s">
-        <v>225</v>
-      </c>
-      <c r="I60" t="s">
-        <v>249</v>
-      </c>
-      <c r="J60" t="s">
-        <v>226</v>
-      </c>
-      <c r="K60" t="s">
-        <v>265</v>
-      </c>
       <c r="M60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N60" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="O60" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P60">
         <v>60</v>
@@ -20794,31 +20791,31 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C61" t="s">
+        <v>265</v>
+      </c>
+      <c r="F61" t="s">
         <v>266</v>
       </c>
-      <c r="F61" t="s">
-        <v>267</v>
-      </c>
       <c r="H61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M61" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N61" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P61">
         <v>61</v>
@@ -20826,37 +20823,37 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B62" t="s">
+        <v>267</v>
+      </c>
+      <c r="C62" t="s">
         <v>268</v>
-      </c>
-      <c r="C62" t="s">
-        <v>269</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
       </c>
       <c r="F62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H62" t="s">
+        <v>219</v>
+      </c>
+      <c r="J62" t="s">
         <v>220</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>221</v>
       </c>
-      <c r="K62" t="s">
-        <v>222</v>
-      </c>
       <c r="M62" t="s">
+        <v>383</v>
+      </c>
+      <c r="N62" t="s">
         <v>384</v>
       </c>
-      <c r="N62" t="s">
-        <v>385</v>
-      </c>
       <c r="O62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P62">
         <v>62</v>
@@ -20864,31 +20861,31 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C63" t="s">
+        <v>270</v>
+      </c>
+      <c r="F63" t="s">
         <v>271</v>
       </c>
-      <c r="F63" t="s">
-        <v>272</v>
-      </c>
       <c r="H63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K63" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M63" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N63" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O63" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P63">
         <v>63</v>
@@ -20896,34 +20893,34 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
       </c>
       <c r="F64" t="s">
+        <v>273</v>
+      </c>
+      <c r="H64" t="s">
         <v>274</v>
       </c>
-      <c r="H64" t="s">
+      <c r="J64" t="s">
+        <v>220</v>
+      </c>
+      <c r="K64" t="s">
         <v>275</v>
       </c>
-      <c r="J64" t="s">
-        <v>221</v>
-      </c>
-      <c r="K64" t="s">
-        <v>276</v>
-      </c>
       <c r="M64" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N64" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P64">
         <v>64</v>
@@ -20931,22 +20928,22 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M65" t="s">
+        <v>374</v>
+      </c>
+      <c r="N65" t="s">
         <v>375</v>
       </c>
-      <c r="N65" t="s">
-        <v>376</v>
-      </c>
       <c r="O65" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P65">
         <v>65</v>
@@ -20954,37 +20951,37 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B66" t="s">
+        <v>277</v>
+      </c>
+      <c r="C66" t="s">
         <v>278</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
+        <v>244</v>
+      </c>
+      <c r="F66" t="s">
         <v>279</v>
       </c>
-      <c r="E66" t="s">
-        <v>245</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="H66" t="s">
         <v>280</v>
-      </c>
-      <c r="H66" t="s">
-        <v>281</v>
       </c>
       <c r="I66" t="s">
         <v>133</v>
       </c>
       <c r="L66" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N66" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O66" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P66">
         <v>66</v>
@@ -20992,34 +20989,34 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C67" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E67" t="s">
         <v>133</v>
       </c>
       <c r="F67" t="s">
+        <v>213</v>
+      </c>
+      <c r="H67" t="s">
         <v>214</v>
-      </c>
-      <c r="H67" t="s">
-        <v>215</v>
       </c>
       <c r="I67" t="s">
         <v>133</v>
       </c>
       <c r="L67" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N67" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P67">
         <v>67</v>
@@ -21027,37 +21024,37 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B68" t="s">
+        <v>284</v>
+      </c>
+      <c r="C68" t="s">
         <v>285</v>
-      </c>
-      <c r="C68" t="s">
-        <v>286</v>
       </c>
       <c r="D68" t="s">
         <v>56</v>
       </c>
       <c r="F68" t="s">
+        <v>286</v>
+      </c>
+      <c r="H68" t="s">
         <v>287</v>
       </c>
-      <c r="H68" t="s">
+      <c r="J68" t="s">
+        <v>225</v>
+      </c>
+      <c r="K68" t="s">
         <v>288</v>
       </c>
-      <c r="J68" t="s">
-        <v>226</v>
-      </c>
-      <c r="K68" t="s">
-        <v>289</v>
-      </c>
       <c r="M68" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N68" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P68">
         <v>68</v>
@@ -21065,31 +21062,31 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C69" t="s">
+        <v>289</v>
+      </c>
+      <c r="F69" t="s">
         <v>290</v>
       </c>
-      <c r="F69" t="s">
-        <v>291</v>
-      </c>
       <c r="H69" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M69" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N69" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O69" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P69">
         <v>69</v>
@@ -21097,34 +21094,34 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C70" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F70" t="s">
+        <v>246</v>
+      </c>
+      <c r="H70" t="s">
         <v>247</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>248</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
+        <v>220</v>
+      </c>
+      <c r="K70" t="s">
         <v>249</v>
       </c>
-      <c r="J70" t="s">
-        <v>221</v>
-      </c>
-      <c r="K70" t="s">
-        <v>250</v>
-      </c>
       <c r="M70" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N70" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O70" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P70">
         <v>70</v>
@@ -21132,31 +21129,31 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C71" t="s">
+        <v>292</v>
+      </c>
+      <c r="F71" t="s">
         <v>293</v>
       </c>
-      <c r="F71" t="s">
-        <v>294</v>
-      </c>
       <c r="H71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N71" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O71" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P71">
         <v>71</v>
@@ -21164,31 +21161,31 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B72" t="s">
+        <v>294</v>
+      </c>
+      <c r="C72" t="s">
         <v>295</v>
       </c>
-      <c r="C72" t="s">
+      <c r="H72" t="s">
         <v>296</v>
       </c>
-      <c r="H72" t="s">
+      <c r="J72" t="s">
         <v>297</v>
       </c>
-      <c r="J72" t="s">
+      <c r="K72" t="s">
         <v>298</v>
       </c>
-      <c r="K72" t="s">
-        <v>299</v>
-      </c>
       <c r="M72" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N72" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="O72" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P72">
         <v>72</v>
@@ -21196,22 +21193,22 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E73" t="s">
         <v>133</v>
       </c>
       <c r="M73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N73" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O73" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P73">
         <v>73</v>
@@ -21219,37 +21216,37 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B74" t="s">
+        <v>300</v>
+      </c>
+      <c r="C74" t="s">
         <v>301</v>
-      </c>
-      <c r="C74" t="s">
-        <v>302</v>
       </c>
       <c r="D74" t="s">
         <v>56</v>
       </c>
       <c r="F74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H74" t="s">
+        <v>224</v>
+      </c>
+      <c r="J74" t="s">
         <v>225</v>
       </c>
-      <c r="J74" t="s">
+      <c r="K74" t="s">
         <v>226</v>
       </c>
-      <c r="K74" t="s">
-        <v>227</v>
-      </c>
       <c r="M74" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N74" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="O74" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P74">
         <v>74</v>
@@ -21257,34 +21254,34 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B75" t="s">
+        <v>302</v>
+      </c>
+      <c r="C75" t="s">
         <v>303</v>
       </c>
-      <c r="C75" t="s">
+      <c r="F75" t="s">
         <v>304</v>
       </c>
-      <c r="F75" t="s">
-        <v>305</v>
-      </c>
       <c r="H75" t="s">
+        <v>224</v>
+      </c>
+      <c r="J75" t="s">
         <v>225</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>226</v>
       </c>
-      <c r="K75" t="s">
-        <v>227</v>
-      </c>
       <c r="M75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N75" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="O75" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P75">
         <v>75</v>
@@ -21292,34 +21289,34 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B76" t="s">
+        <v>305</v>
+      </c>
+      <c r="C76" t="s">
         <v>306</v>
-      </c>
-      <c r="C76" t="s">
-        <v>307</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
       </c>
       <c r="H76" t="s">
+        <v>307</v>
+      </c>
+      <c r="J76" t="s">
+        <v>220</v>
+      </c>
+      <c r="K76" t="s">
         <v>308</v>
       </c>
-      <c r="J76" t="s">
-        <v>221</v>
-      </c>
-      <c r="K76" t="s">
-        <v>309</v>
-      </c>
       <c r="M76" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N76" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P76">
         <v>76</v>
@@ -21327,37 +21324,37 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B77" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" t="s">
         <v>310</v>
-      </c>
-      <c r="C77" t="s">
-        <v>311</v>
       </c>
       <c r="D77" t="s">
         <v>56</v>
       </c>
       <c r="F77" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H77" t="s">
+        <v>224</v>
+      </c>
+      <c r="J77" t="s">
         <v>225</v>
       </c>
-      <c r="J77" t="s">
+      <c r="K77" t="s">
         <v>226</v>
       </c>
-      <c r="K77" t="s">
-        <v>227</v>
-      </c>
       <c r="M77" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N77" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="O77" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P77">
         <v>77</v>
@@ -21370,6 +21367,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA58F2CACE833A4EAC3C2718D7553EBC" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="70bd391f7da495450ffbbb84ed005d64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7880897e-52c6-4ffd-85c8-5c6950347fc0" xmlns:ns4="8c824e80-41b8-4a07-a4d9-9d9814734933" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff4fc1df527a05bf252a4f5512a06a4f" ns3:_="" ns4:_="">
     <xsd:import namespace="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
@@ -21566,12 +21569,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -21582,6 +21579,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DB8A40F-A4F0-4420-9B0D-425E1B516684}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8c824e80-41b8-4a07-a4d9-9d9814734933"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB43457-B126-4564-BEE0-23045A6D0196}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21600,23 +21614,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DB8A40F-A4F0-4420-9B0D-425E1B516684}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8c824e80-41b8-4a07-a4d9-9d9814734933"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{507E2990-634F-4225-AAE8-6587B51CDB5B}">
   <ds:schemaRefs>

</xml_diff>